<commit_message>
fix error web rep kis
</commit_message>
<xml_diff>
--- a/Documents/График внедрения RailWay.xlsx
+++ b/Documents/График внедрения RailWay.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work MPP\Логистика\RailWay\Внедрение АСКВД\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Мои документы\Visual Studio 2013\Projects\Work\New RailWay\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1373,18 +1373,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1394,9 +1397,6 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1412,25 +1412,55 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1439,12 +1469,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1463,31 +1487,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1773,7 +1773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B13" sqref="B13:B16"/>
     </sheetView>
   </sheetViews>
@@ -1916,10 +1916,10 @@
       <c r="E6" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="58" t="s">
+      <c r="F6" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="G6" s="58" t="s">
+      <c r="G6" s="56" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1935,57 +1935,57 @@
       <c r="E7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="59"/>
-      <c r="G7" s="59"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="56">
+      <c r="A8" s="59">
         <v>6</v>
       </c>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="60" t="s">
         <v>62</v>
       </c>
       <c r="C8" s="64" t="s">
         <v>66</v>
       </c>
-      <c r="D8" s="58" t="s">
+      <c r="D8" s="56" t="s">
         <v>84</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="G8" s="60" t="s">
+      <c r="G8" s="61" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="56"/>
-      <c r="B9" s="57"/>
+      <c r="A9" s="59"/>
+      <c r="B9" s="60"/>
       <c r="C9" s="64"/>
-      <c r="D9" s="63"/>
+      <c r="D9" s="57"/>
       <c r="E9" s="13"/>
       <c r="F9" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="61"/>
+      <c r="G9" s="62"/>
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="56"/>
-      <c r="B10" s="57"/>
+      <c r="A10" s="59"/>
+      <c r="B10" s="60"/>
       <c r="C10" s="64"/>
-      <c r="D10" s="59"/>
+      <c r="D10" s="58"/>
       <c r="E10" s="13"/>
       <c r="F10" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="G10" s="62"/>
+      <c r="G10" s="63"/>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="56">
+      <c r="A11" s="59">
         <v>7</v>
       </c>
-      <c r="B11" s="57" t="s">
+      <c r="B11" s="60" t="s">
         <v>61</v>
       </c>
       <c r="C11" s="51" t="s">
@@ -1995,16 +1995,16 @@
         <v>85</v>
       </c>
       <c r="E11" s="13"/>
-      <c r="F11" s="58" t="s">
+      <c r="F11" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="G11" s="58" t="s">
+      <c r="G11" s="56" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="56"/>
-      <c r="B12" s="57"/>
+      <c r="A12" s="59"/>
+      <c r="B12" s="60"/>
       <c r="C12" s="51" t="s">
         <v>102</v>
       </c>
@@ -2012,14 +2012,14 @@
         <v>87</v>
       </c>
       <c r="E12" s="13"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="59"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="58"/>
     </row>
     <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="56">
+      <c r="A13" s="59">
         <v>8</v>
       </c>
-      <c r="B13" s="57" t="s">
+      <c r="B13" s="60" t="s">
         <v>155</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -2029,16 +2029,16 @@
         <v>92</v>
       </c>
       <c r="E13" s="13"/>
-      <c r="F13" s="58" t="s">
+      <c r="F13" s="56" t="s">
         <v>154</v>
       </c>
-      <c r="G13" s="58" t="s">
+      <c r="G13" s="56" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="56"/>
-      <c r="B14" s="57"/>
+      <c r="A14" s="59"/>
+      <c r="B14" s="60"/>
       <c r="C14" s="11" t="s">
         <v>104</v>
       </c>
@@ -2046,12 +2046,12 @@
         <v>93</v>
       </c>
       <c r="E14" s="20"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="63"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="57"/>
     </row>
     <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="56"/>
-      <c r="B15" s="57"/>
+      <c r="A15" s="59"/>
+      <c r="B15" s="60"/>
       <c r="C15" s="11" t="s">
         <v>105</v>
       </c>
@@ -2059,12 +2059,12 @@
         <v>94</v>
       </c>
       <c r="E15" s="20"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="63"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
     </row>
     <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="56"/>
-      <c r="B16" s="57"/>
+      <c r="A16" s="59"/>
+      <c r="B16" s="60"/>
       <c r="C16" s="11" t="s">
         <v>95</v>
       </c>
@@ -2072,11 +2072,12 @@
         <v>96</v>
       </c>
       <c r="E16" s="20"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="59"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B6:B7"/>
     <mergeCell ref="D8:D10"/>
     <mergeCell ref="A13:A16"/>
     <mergeCell ref="B13:B16"/>
@@ -2093,7 +2094,6 @@
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="C8:C10"/>
     <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1"/>
@@ -2103,7 +2103,7 @@
     <hyperlink ref="E7" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" scale="58" orientation="landscape" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -2164,16 +2164,16 @@
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="92">
+      <c r="A2" s="75">
         <v>1</v>
       </c>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="72" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="71" t="s">
+      <c r="C2" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="D2" s="71" t="s">
+      <c r="D2" s="72" t="s">
         <v>122</v>
       </c>
       <c r="E2" s="22" t="s">
@@ -2182,10 +2182,10 @@
       <c r="F2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="73">
+      <c r="G2" s="84">
         <v>1</v>
       </c>
-      <c r="H2" s="73" t="s">
+      <c r="H2" s="84" t="s">
         <v>0</v>
       </c>
       <c r="I2" s="26"/>
@@ -2198,18 +2198,18 @@
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="93"/>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
+      <c r="A3" s="76"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
       <c r="E3" s="9" t="s">
         <v>21</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
       <c r="I3" s="27"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -2220,18 +2220,18 @@
       <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="93"/>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
+      <c r="A4" s="76"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
       <c r="E4" s="9" t="s">
         <v>22</v>
       </c>
       <c r="F4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
       <c r="I4" s="27"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -2242,10 +2242,10 @@
       <c r="P4" s="1"/>
     </row>
     <row r="5" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="93"/>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69" t="s">
+      <c r="A5" s="76"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73" t="s">
         <v>123</v>
       </c>
       <c r="E5" s="11" t="s">
@@ -2254,10 +2254,10 @@
       <c r="F5" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="74">
-        <v>0</v>
-      </c>
-      <c r="H5" s="56" t="s">
+      <c r="G5" s="85">
+        <v>0</v>
+      </c>
+      <c r="H5" s="59" t="s">
         <v>124</v>
       </c>
       <c r="I5" s="27"/>
@@ -2270,18 +2270,18 @@
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="1:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="94"/>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
+      <c r="A6" s="77"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
       <c r="E6" s="24" t="s">
         <v>77</v>
       </c>
       <c r="F6" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75"/>
+      <c r="G6" s="94"/>
+      <c r="H6" s="94"/>
       <c r="I6" s="28"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -2292,16 +2292,16 @@
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="92">
+      <c r="A7" s="75">
         <v>2</v>
       </c>
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="71" t="s">
+      <c r="C7" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="71" t="s">
+      <c r="D7" s="72" t="s">
         <v>129</v>
       </c>
       <c r="E7" s="22" t="s">
@@ -2310,33 +2310,33 @@
       <c r="F7" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="73">
+      <c r="G7" s="84">
         <v>1</v>
       </c>
-      <c r="H7" s="76" t="s">
+      <c r="H7" s="86" t="s">
         <v>0</v>
       </c>
       <c r="I7" s="29"/>
     </row>
     <row r="8" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="93"/>
-      <c r="B8" s="69"/>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69"/>
+      <c r="A8" s="76"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
       <c r="E8" s="9" t="s">
         <v>108</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="74"/>
-      <c r="H8" s="77"/>
+      <c r="G8" s="85"/>
+      <c r="H8" s="87"/>
       <c r="I8" s="30"/>
     </row>
     <row r="9" spans="1:16" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="94"/>
-      <c r="B9" s="72"/>
-      <c r="C9" s="72"/>
+      <c r="A9" s="77"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="74"/>
       <c r="D9" s="38" t="s">
         <v>127</v>
       </c>
@@ -2357,16 +2357,16 @@
       </c>
     </row>
     <row r="10" spans="1:16" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="92">
+      <c r="A10" s="75">
         <v>3</v>
       </c>
-      <c r="B10" s="71" t="s">
+      <c r="B10" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="71" t="s">
+      <c r="C10" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="78" t="s">
+      <c r="D10" s="79" t="s">
         <v>129</v>
       </c>
       <c r="E10" s="22" t="s">
@@ -2375,50 +2375,50 @@
       <c r="F10" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="G10" s="80">
+      <c r="G10" s="88">
         <v>1</v>
       </c>
-      <c r="H10" s="83" t="s">
+      <c r="H10" s="91" t="s">
         <v>0</v>
       </c>
       <c r="I10" s="29"/>
     </row>
     <row r="11" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="93"/>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="79"/>
+      <c r="A11" s="76"/>
+      <c r="B11" s="73"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="80"/>
       <c r="E11" s="9" t="s">
         <v>6</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G11" s="81"/>
-      <c r="H11" s="84"/>
+      <c r="G11" s="89"/>
+      <c r="H11" s="92"/>
       <c r="I11" s="30"/>
     </row>
     <row r="12" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="93"/>
-      <c r="B12" s="69"/>
-      <c r="C12" s="69"/>
-      <c r="D12" s="79"/>
+      <c r="A12" s="76"/>
+      <c r="B12" s="73"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="80"/>
       <c r="E12" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F12" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G12" s="82"/>
-      <c r="H12" s="85"/>
+      <c r="G12" s="90"/>
+      <c r="H12" s="93"/>
       <c r="I12" s="41" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="94"/>
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
+      <c r="A13" s="77"/>
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
       <c r="D13" s="38" t="s">
         <v>127</v>
       </c>
@@ -2439,16 +2439,16 @@
       </c>
     </row>
     <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="86" t="s">
+      <c r="A14" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="71" t="s">
+      <c r="B14" s="72" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="71" t="s">
+      <c r="C14" s="72" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="78" t="s">
+      <c r="D14" s="79" t="s">
         <v>129</v>
       </c>
       <c r="E14" s="22" t="s">
@@ -2457,82 +2457,82 @@
       <c r="F14" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="71" t="s">
+      <c r="G14" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="71" t="s">
+      <c r="H14" s="72" t="s">
         <v>0</v>
       </c>
       <c r="I14" s="29"/>
     </row>
     <row r="15" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="87"/>
-      <c r="B15" s="69"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="79"/>
+      <c r="A15" s="70"/>
+      <c r="B15" s="73"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="80"/>
       <c r="E15" s="9" t="s">
         <v>111</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G15" s="69"/>
-      <c r="H15" s="69"/>
+      <c r="G15" s="73"/>
+      <c r="H15" s="73"/>
       <c r="I15" s="41" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="87"/>
-      <c r="B16" s="69"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="79"/>
+      <c r="A16" s="70"/>
+      <c r="B16" s="73"/>
+      <c r="C16" s="73"/>
+      <c r="D16" s="80"/>
       <c r="E16" s="9" t="s">
         <v>112</v>
       </c>
       <c r="F16" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G16" s="69"/>
-      <c r="H16" s="69"/>
+      <c r="G16" s="73"/>
+      <c r="H16" s="73"/>
       <c r="I16" s="41"/>
     </row>
     <row r="17" spans="1:16" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="87"/>
-      <c r="B17" s="69"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="79"/>
+      <c r="A17" s="70"/>
+      <c r="B17" s="73"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="80"/>
       <c r="E17" s="9" t="s">
         <v>17</v>
       </c>
       <c r="F17" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G17" s="69"/>
-      <c r="H17" s="69"/>
+      <c r="G17" s="73"/>
+      <c r="H17" s="73"/>
       <c r="I17" s="41"/>
     </row>
     <row r="18" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="87"/>
-      <c r="B18" s="69"/>
-      <c r="C18" s="69"/>
-      <c r="D18" s="79"/>
+      <c r="A18" s="70"/>
+      <c r="B18" s="73"/>
+      <c r="C18" s="73"/>
+      <c r="D18" s="80"/>
       <c r="E18" s="9" t="s">
         <v>13</v>
       </c>
       <c r="F18" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G18" s="69"/>
-      <c r="H18" s="69"/>
+      <c r="G18" s="73"/>
+      <c r="H18" s="73"/>
       <c r="I18" s="41" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="91"/>
-      <c r="B19" s="70"/>
-      <c r="C19" s="70"/>
+      <c r="A19" s="71"/>
+      <c r="B19" s="78"/>
+      <c r="C19" s="78"/>
       <c r="D19" s="39" t="s">
         <v>127</v>
       </c>
@@ -2551,16 +2551,16 @@
       <c r="I19" s="44"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="86" t="s">
+      <c r="A20" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="71" t="s">
+      <c r="B20" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="C20" s="71" t="s">
+      <c r="C20" s="72" t="s">
         <v>161</v>
       </c>
-      <c r="D20" s="71" t="s">
+      <c r="D20" s="72" t="s">
         <v>131</v>
       </c>
       <c r="E20" s="22" t="s">
@@ -2569,10 +2569,10 @@
       <c r="F20" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="G20" s="71" t="s">
+      <c r="G20" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="71" t="s">
+      <c r="H20" s="72" t="s">
         <v>0</v>
       </c>
       <c r="I20" s="26"/>
@@ -2585,18 +2585,18 @@
       <c r="P20" s="1"/>
     </row>
     <row r="21" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="87"/>
-      <c r="B21" s="69"/>
-      <c r="C21" s="69"/>
-      <c r="D21" s="69"/>
+      <c r="A21" s="70"/>
+      <c r="B21" s="73"/>
+      <c r="C21" s="73"/>
+      <c r="D21" s="73"/>
       <c r="E21" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G21" s="69"/>
-      <c r="H21" s="69"/>
+      <c r="G21" s="73"/>
+      <c r="H21" s="73"/>
       <c r="I21" s="27"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -2607,18 +2607,18 @@
       <c r="P21" s="1"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="87"/>
-      <c r="B22" s="69"/>
-      <c r="C22" s="69"/>
-      <c r="D22" s="69"/>
+      <c r="A22" s="70"/>
+      <c r="B22" s="73"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="73"/>
       <c r="E22" s="9" t="s">
         <v>26</v>
       </c>
       <c r="F22" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G22" s="69"/>
-      <c r="H22" s="69"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="73"/>
       <c r="I22" s="27"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -2629,18 +2629,18 @@
       <c r="P22" s="1"/>
     </row>
     <row r="23" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="87"/>
-      <c r="B23" s="69"/>
-      <c r="C23" s="69"/>
-      <c r="D23" s="69"/>
+      <c r="A23" s="70"/>
+      <c r="B23" s="73"/>
+      <c r="C23" s="73"/>
+      <c r="D23" s="73"/>
       <c r="E23" s="9" t="s">
         <v>28</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G23" s="69"/>
-      <c r="H23" s="69"/>
+      <c r="G23" s="73"/>
+      <c r="H23" s="73"/>
       <c r="I23" s="27"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -2651,18 +2651,18 @@
       <c r="P23" s="1"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="87"/>
-      <c r="B24" s="69"/>
-      <c r="C24" s="69"/>
-      <c r="D24" s="69"/>
+      <c r="A24" s="70"/>
+      <c r="B24" s="73"/>
+      <c r="C24" s="73"/>
+      <c r="D24" s="73"/>
       <c r="E24" s="9" t="s">
         <v>27</v>
       </c>
       <c r="F24" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G24" s="69"/>
-      <c r="H24" s="69"/>
+      <c r="G24" s="73"/>
+      <c r="H24" s="73"/>
       <c r="I24" s="27"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -2673,10 +2673,10 @@
       <c r="P24" s="1"/>
     </row>
     <row r="25" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="87"/>
-      <c r="B25" s="69"/>
-      <c r="C25" s="69"/>
-      <c r="D25" s="69" t="s">
+      <c r="A25" s="70"/>
+      <c r="B25" s="73"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="73" t="s">
         <v>133</v>
       </c>
       <c r="E25" s="9" t="s">
@@ -2685,109 +2685,109 @@
       <c r="F25" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G25" s="69" t="s">
+      <c r="G25" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="H25" s="69" t="s">
+      <c r="H25" s="73" t="s">
         <v>0</v>
       </c>
       <c r="I25" s="41"/>
     </row>
     <row r="26" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="87"/>
-      <c r="B26" s="69"/>
-      <c r="C26" s="69"/>
-      <c r="D26" s="69"/>
+      <c r="A26" s="70"/>
+      <c r="B26" s="73"/>
+      <c r="C26" s="73"/>
+      <c r="D26" s="73"/>
       <c r="E26" s="9" t="s">
         <v>34</v>
       </c>
       <c r="F26" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G26" s="69"/>
-      <c r="H26" s="69"/>
+      <c r="G26" s="73"/>
+      <c r="H26" s="73"/>
       <c r="I26" s="27"/>
     </row>
     <row r="27" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="87"/>
-      <c r="B27" s="69"/>
-      <c r="C27" s="69"/>
-      <c r="D27" s="69"/>
+      <c r="A27" s="70"/>
+      <c r="B27" s="73"/>
+      <c r="C27" s="73"/>
+      <c r="D27" s="73"/>
       <c r="E27" s="9" t="s">
         <v>35</v>
       </c>
       <c r="F27" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G27" s="69"/>
-      <c r="H27" s="69"/>
+      <c r="G27" s="73"/>
+      <c r="H27" s="73"/>
       <c r="I27" s="27"/>
     </row>
     <row r="28" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="87"/>
-      <c r="B28" s="69"/>
-      <c r="C28" s="69"/>
-      <c r="D28" s="69"/>
+      <c r="A28" s="70"/>
+      <c r="B28" s="73"/>
+      <c r="C28" s="73"/>
+      <c r="D28" s="73"/>
       <c r="E28" s="9" t="s">
         <v>56</v>
       </c>
       <c r="F28" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G28" s="69"/>
-      <c r="H28" s="69"/>
+      <c r="G28" s="73"/>
+      <c r="H28" s="73"/>
       <c r="I28" s="27"/>
     </row>
     <row r="29" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="87"/>
-      <c r="B29" s="69"/>
-      <c r="C29" s="69"/>
-      <c r="D29" s="69"/>
+      <c r="A29" s="70"/>
+      <c r="B29" s="73"/>
+      <c r="C29" s="73"/>
+      <c r="D29" s="73"/>
       <c r="E29" s="9" t="s">
         <v>36</v>
       </c>
       <c r="F29" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G29" s="69"/>
-      <c r="H29" s="69"/>
+      <c r="G29" s="73"/>
+      <c r="H29" s="73"/>
       <c r="I29" s="27"/>
     </row>
     <row r="30" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="87"/>
-      <c r="B30" s="69"/>
-      <c r="C30" s="69"/>
-      <c r="D30" s="69"/>
+      <c r="A30" s="70"/>
+      <c r="B30" s="73"/>
+      <c r="C30" s="73"/>
+      <c r="D30" s="73"/>
       <c r="E30" s="9" t="s">
         <v>37</v>
       </c>
       <c r="F30" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G30" s="69"/>
-      <c r="H30" s="69"/>
+      <c r="G30" s="73"/>
+      <c r="H30" s="73"/>
       <c r="I30" s="27"/>
     </row>
     <row r="31" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="87"/>
-      <c r="B31" s="69"/>
-      <c r="C31" s="69"/>
-      <c r="D31" s="69"/>
+      <c r="A31" s="70"/>
+      <c r="B31" s="73"/>
+      <c r="C31" s="73"/>
+      <c r="D31" s="73"/>
       <c r="E31" s="9" t="s">
         <v>38</v>
       </c>
       <c r="F31" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G31" s="69"/>
-      <c r="H31" s="69"/>
+      <c r="G31" s="73"/>
+      <c r="H31" s="73"/>
       <c r="I31" s="27"/>
     </row>
     <row r="32" spans="1:16" ht="75" x14ac:dyDescent="0.25">
-      <c r="A32" s="87"/>
-      <c r="B32" s="69"/>
-      <c r="C32" s="69"/>
-      <c r="D32" s="69" t="s">
+      <c r="A32" s="70"/>
+      <c r="B32" s="73"/>
+      <c r="C32" s="73"/>
+      <c r="D32" s="73" t="s">
         <v>132</v>
       </c>
       <c r="E32" s="8" t="s">
@@ -2796,36 +2796,36 @@
       <c r="F32" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="G32" s="69" t="s">
+      <c r="G32" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="H32" s="69" t="s">
+      <c r="H32" s="73" t="s">
         <v>82</v>
       </c>
       <c r="I32" s="27"/>
     </row>
     <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="87"/>
-      <c r="B33" s="69"/>
-      <c r="C33" s="69"/>
-      <c r="D33" s="69"/>
+      <c r="A33" s="70"/>
+      <c r="B33" s="73"/>
+      <c r="C33" s="73"/>
+      <c r="D33" s="73"/>
       <c r="E33" s="10" t="s">
         <v>43</v>
       </c>
       <c r="F33" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G33" s="69"/>
-      <c r="H33" s="69"/>
+      <c r="G33" s="73"/>
+      <c r="H33" s="73"/>
       <c r="I33" s="41" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="87"/>
-      <c r="B34" s="69"/>
-      <c r="C34" s="69"/>
-      <c r="D34" s="69" t="s">
+      <c r="A34" s="70"/>
+      <c r="B34" s="73"/>
+      <c r="C34" s="73"/>
+      <c r="D34" s="73" t="s">
         <v>135</v>
       </c>
       <c r="E34" s="10" t="s">
@@ -2834,10 +2834,10 @@
       <c r="F34" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G34" s="69" t="s">
+      <c r="G34" s="73" t="s">
         <v>134</v>
       </c>
-      <c r="H34" s="69" t="s">
+      <c r="H34" s="73" t="s">
         <v>85</v>
       </c>
       <c r="I34" s="41" t="s">
@@ -2845,115 +2845,115 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="87"/>
-      <c r="B35" s="69"/>
-      <c r="C35" s="69"/>
-      <c r="D35" s="69"/>
+      <c r="A35" s="70"/>
+      <c r="B35" s="73"/>
+      <c r="C35" s="73"/>
+      <c r="D35" s="73"/>
       <c r="E35" s="10" t="s">
         <v>39</v>
       </c>
       <c r="F35" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G35" s="69"/>
-      <c r="H35" s="69"/>
+      <c r="G35" s="73"/>
+      <c r="H35" s="73"/>
       <c r="I35" s="41"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="87"/>
-      <c r="B36" s="69"/>
-      <c r="C36" s="69"/>
-      <c r="D36" s="69"/>
+      <c r="A36" s="70"/>
+      <c r="B36" s="73"/>
+      <c r="C36" s="73"/>
+      <c r="D36" s="73"/>
       <c r="E36" s="10" t="s">
         <v>114</v>
       </c>
       <c r="F36" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G36" s="69"/>
-      <c r="H36" s="69"/>
+      <c r="G36" s="73"/>
+      <c r="H36" s="73"/>
       <c r="I36" s="41"/>
     </row>
     <row r="37" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="87"/>
-      <c r="B37" s="69"/>
-      <c r="C37" s="69"/>
-      <c r="D37" s="69"/>
+      <c r="A37" s="70"/>
+      <c r="B37" s="73"/>
+      <c r="C37" s="73"/>
+      <c r="D37" s="73"/>
       <c r="E37" s="10" t="s">
         <v>115</v>
       </c>
       <c r="F37" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G37" s="69"/>
-      <c r="H37" s="69"/>
+      <c r="G37" s="73"/>
+      <c r="H37" s="73"/>
       <c r="I37" s="41"/>
     </row>
     <row r="38" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="87"/>
-      <c r="B38" s="69"/>
-      <c r="C38" s="69"/>
-      <c r="D38" s="69"/>
+      <c r="A38" s="70"/>
+      <c r="B38" s="73"/>
+      <c r="C38" s="73"/>
+      <c r="D38" s="73"/>
       <c r="E38" s="10" t="s">
         <v>116</v>
       </c>
       <c r="F38" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G38" s="69"/>
-      <c r="H38" s="69"/>
+      <c r="G38" s="73"/>
+      <c r="H38" s="73"/>
       <c r="I38" s="41"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="87"/>
-      <c r="B39" s="69"/>
-      <c r="C39" s="69"/>
-      <c r="D39" s="69"/>
+      <c r="A39" s="70"/>
+      <c r="B39" s="73"/>
+      <c r="C39" s="73"/>
+      <c r="D39" s="73"/>
       <c r="E39" s="10" t="s">
         <v>45</v>
       </c>
       <c r="F39" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G39" s="69"/>
-      <c r="H39" s="69"/>
+      <c r="G39" s="73"/>
+      <c r="H39" s="73"/>
       <c r="I39" s="41"/>
     </row>
     <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="87"/>
-      <c r="B40" s="69"/>
-      <c r="C40" s="69"/>
-      <c r="D40" s="69"/>
+      <c r="A40" s="70"/>
+      <c r="B40" s="73"/>
+      <c r="C40" s="73"/>
+      <c r="D40" s="73"/>
       <c r="E40" s="11" t="s">
         <v>46</v>
       </c>
       <c r="F40" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="G40" s="69"/>
-      <c r="H40" s="69"/>
+      <c r="G40" s="73"/>
+      <c r="H40" s="73"/>
       <c r="I40" s="41"/>
     </row>
     <row r="41" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A41" s="87"/>
-      <c r="B41" s="69"/>
-      <c r="C41" s="69"/>
-      <c r="D41" s="69"/>
+      <c r="A41" s="70"/>
+      <c r="B41" s="73"/>
+      <c r="C41" s="73"/>
+      <c r="D41" s="73"/>
       <c r="E41" s="11" t="s">
         <v>57</v>
       </c>
       <c r="F41" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="G41" s="69"/>
-      <c r="H41" s="69"/>
+      <c r="G41" s="73"/>
+      <c r="H41" s="73"/>
       <c r="I41" s="41"/>
     </row>
     <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="87"/>
-      <c r="B42" s="69"/>
-      <c r="C42" s="69"/>
-      <c r="D42" s="69" t="s">
+      <c r="A42" s="70"/>
+      <c r="B42" s="73"/>
+      <c r="C42" s="73"/>
+      <c r="D42" s="73" t="s">
         <v>136</v>
       </c>
       <c r="E42" s="9" t="s">
@@ -2962,49 +2962,49 @@
       <c r="F42" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G42" s="69" t="s">
+      <c r="G42" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="H42" s="69" t="s">
+      <c r="H42" s="73" t="s">
         <v>0</v>
       </c>
       <c r="I42" s="41"/>
     </row>
     <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="87"/>
-      <c r="B43" s="69"/>
-      <c r="C43" s="69"/>
-      <c r="D43" s="69"/>
+      <c r="A43" s="70"/>
+      <c r="B43" s="73"/>
+      <c r="C43" s="73"/>
+      <c r="D43" s="73"/>
       <c r="E43" s="9" t="s">
         <v>113</v>
       </c>
       <c r="F43" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G43" s="69"/>
-      <c r="H43" s="69"/>
+      <c r="G43" s="73"/>
+      <c r="H43" s="73"/>
       <c r="I43" s="27"/>
     </row>
     <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="87"/>
-      <c r="B44" s="69"/>
-      <c r="C44" s="69"/>
-      <c r="D44" s="69"/>
+      <c r="A44" s="70"/>
+      <c r="B44" s="73"/>
+      <c r="C44" s="73"/>
+      <c r="D44" s="73"/>
       <c r="E44" s="9" t="s">
         <v>53</v>
       </c>
       <c r="F44" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G44" s="69"/>
-      <c r="H44" s="69"/>
+      <c r="G44" s="73"/>
+      <c r="H44" s="73"/>
       <c r="I44" s="27"/>
     </row>
     <row r="45" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A45" s="87"/>
-      <c r="B45" s="69"/>
-      <c r="C45" s="69"/>
-      <c r="D45" s="69" t="s">
+      <c r="A45" s="70"/>
+      <c r="B45" s="73"/>
+      <c r="C45" s="73"/>
+      <c r="D45" s="73" t="s">
         <v>137</v>
       </c>
       <c r="E45" s="10" t="s">
@@ -3013,36 +3013,36 @@
       <c r="F45" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G45" s="69" t="s">
+      <c r="G45" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="H45" s="69" t="s">
+      <c r="H45" s="73" t="s">
         <v>82</v>
       </c>
       <c r="I45" s="27"/>
     </row>
     <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="87"/>
-      <c r="B46" s="69"/>
-      <c r="C46" s="69"/>
-      <c r="D46" s="69"/>
+      <c r="A46" s="70"/>
+      <c r="B46" s="73"/>
+      <c r="C46" s="73"/>
+      <c r="D46" s="73"/>
       <c r="E46" s="10" t="s">
         <v>52</v>
       </c>
       <c r="F46" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G46" s="69"/>
-      <c r="H46" s="69"/>
+      <c r="G46" s="73"/>
+      <c r="H46" s="73"/>
       <c r="I46" s="41" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="87"/>
-      <c r="B47" s="69"/>
-      <c r="C47" s="69"/>
-      <c r="D47" s="69" t="s">
+      <c r="A47" s="70"/>
+      <c r="B47" s="73"/>
+      <c r="C47" s="73"/>
+      <c r="D47" s="73" t="s">
         <v>162</v>
       </c>
       <c r="E47" s="11" t="s">
@@ -3051,10 +3051,10 @@
       <c r="F47" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="G47" s="69" t="s">
+      <c r="G47" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="H47" s="69" t="s">
+      <c r="H47" s="73" t="s">
         <v>85</v>
       </c>
       <c r="I47" s="41" t="s">
@@ -3062,46 +3062,46 @@
       </c>
     </row>
     <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="87"/>
-      <c r="B48" s="69"/>
-      <c r="C48" s="69"/>
-      <c r="D48" s="69"/>
+      <c r="A48" s="70"/>
+      <c r="B48" s="73"/>
+      <c r="C48" s="73"/>
+      <c r="D48" s="73"/>
       <c r="E48" s="10" t="s">
         <v>138</v>
       </c>
       <c r="F48" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G48" s="69"/>
-      <c r="H48" s="69"/>
+      <c r="G48" s="73"/>
+      <c r="H48" s="73"/>
       <c r="I48" s="41"/>
     </row>
     <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="91"/>
-      <c r="B49" s="70"/>
-      <c r="C49" s="70"/>
-      <c r="D49" s="70"/>
+      <c r="A49" s="71"/>
+      <c r="B49" s="78"/>
+      <c r="C49" s="78"/>
+      <c r="D49" s="78"/>
       <c r="E49" s="42" t="s">
         <v>139</v>
       </c>
       <c r="F49" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="G49" s="70"/>
-      <c r="H49" s="70"/>
+      <c r="G49" s="78"/>
+      <c r="H49" s="78"/>
       <c r="I49" s="46"/>
     </row>
     <row r="50" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A50" s="86" t="s">
+      <c r="A50" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="B50" s="71" t="s">
+      <c r="B50" s="72" t="s">
         <v>140</v>
       </c>
-      <c r="C50" s="71" t="s">
+      <c r="C50" s="72" t="s">
         <v>163</v>
       </c>
-      <c r="D50" s="71" t="s">
+      <c r="D50" s="72" t="s">
         <v>141</v>
       </c>
       <c r="E50" s="47" t="s">
@@ -3110,49 +3110,49 @@
       <c r="F50" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="G50" s="71" t="s">
+      <c r="G50" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="H50" s="71" t="s">
+      <c r="H50" s="72" t="s">
         <v>84</v>
       </c>
       <c r="I50" s="49"/>
     </row>
     <row r="51" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A51" s="87"/>
-      <c r="B51" s="69"/>
-      <c r="C51" s="69"/>
-      <c r="D51" s="69"/>
+      <c r="A51" s="70"/>
+      <c r="B51" s="73"/>
+      <c r="C51" s="73"/>
+      <c r="D51" s="73"/>
       <c r="E51" s="11" t="s">
         <v>48</v>
       </c>
       <c r="F51" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="G51" s="69"/>
-      <c r="H51" s="69"/>
+      <c r="G51" s="73"/>
+      <c r="H51" s="73"/>
       <c r="I51" s="27"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="87"/>
-      <c r="B52" s="69"/>
-      <c r="C52" s="69"/>
-      <c r="D52" s="69"/>
+      <c r="A52" s="70"/>
+      <c r="B52" s="73"/>
+      <c r="C52" s="73"/>
+      <c r="D52" s="73"/>
       <c r="E52" s="11" t="s">
         <v>142</v>
       </c>
       <c r="F52" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="G52" s="69"/>
-      <c r="H52" s="69"/>
+      <c r="G52" s="73"/>
+      <c r="H52" s="73"/>
       <c r="I52" s="27"/>
     </row>
     <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="87"/>
-      <c r="B53" s="69"/>
-      <c r="C53" s="69"/>
-      <c r="D53" s="69" t="s">
+      <c r="A53" s="70"/>
+      <c r="B53" s="73"/>
+      <c r="C53" s="73"/>
+      <c r="D53" s="73" t="s">
         <v>62</v>
       </c>
       <c r="E53" s="11" t="s">
@@ -3161,82 +3161,82 @@
       <c r="F53" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="G53" s="69" t="s">
+      <c r="G53" s="73" t="s">
         <v>80</v>
       </c>
-      <c r="H53" s="69" t="s">
+      <c r="H53" s="73" t="s">
         <v>118</v>
       </c>
       <c r="I53" s="41"/>
     </row>
     <row r="54" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A54" s="87"/>
-      <c r="B54" s="69"/>
-      <c r="C54" s="69"/>
-      <c r="D54" s="69"/>
+      <c r="A54" s="70"/>
+      <c r="B54" s="73"/>
+      <c r="C54" s="73"/>
+      <c r="D54" s="73"/>
       <c r="E54" s="11" t="s">
         <v>70</v>
       </c>
       <c r="F54" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="G54" s="69"/>
-      <c r="H54" s="69"/>
+      <c r="G54" s="73"/>
+      <c r="H54" s="73"/>
       <c r="I54" s="27"/>
     </row>
     <row r="55" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A55" s="87"/>
-      <c r="B55" s="69"/>
-      <c r="C55" s="69"/>
-      <c r="D55" s="69"/>
+      <c r="A55" s="70"/>
+      <c r="B55" s="73"/>
+      <c r="C55" s="73"/>
+      <c r="D55" s="73"/>
       <c r="E55" s="11" t="s">
         <v>72</v>
       </c>
       <c r="F55" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="G55" s="69"/>
-      <c r="H55" s="69"/>
+      <c r="G55" s="73"/>
+      <c r="H55" s="73"/>
       <c r="I55" s="27"/>
     </row>
     <row r="56" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A56" s="87"/>
-      <c r="B56" s="69"/>
-      <c r="C56" s="69"/>
-      <c r="D56" s="69"/>
+      <c r="A56" s="70"/>
+      <c r="B56" s="73"/>
+      <c r="C56" s="73"/>
+      <c r="D56" s="73"/>
       <c r="E56" s="11" t="s">
         <v>71</v>
       </c>
       <c r="F56" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="G56" s="69"/>
-      <c r="H56" s="69"/>
+      <c r="G56" s="73"/>
+      <c r="H56" s="73"/>
       <c r="I56" s="27"/>
     </row>
     <row r="57" spans="1:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="88"/>
-      <c r="B57" s="72"/>
-      <c r="C57" s="72"/>
-      <c r="D57" s="72"/>
+      <c r="A57" s="81"/>
+      <c r="B57" s="74"/>
+      <c r="C57" s="74"/>
+      <c r="D57" s="74"/>
       <c r="E57" s="24" t="s">
         <v>73</v>
       </c>
       <c r="F57" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="G57" s="72"/>
-      <c r="H57" s="72"/>
+      <c r="G57" s="74"/>
+      <c r="H57" s="74"/>
       <c r="I57" s="28"/>
     </row>
     <row r="58" spans="1:9" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="90" t="s">
+      <c r="A58" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="B58" s="89" t="s">
+      <c r="B58" s="82" t="s">
         <v>61</v>
       </c>
-      <c r="C58" s="89" t="s">
+      <c r="C58" s="82" t="s">
         <v>157</v>
       </c>
       <c r="D58" s="36" t="s">
@@ -3248,18 +3248,18 @@
       <c r="F58" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="G58" s="89" t="s">
+      <c r="G58" s="82" t="s">
         <v>80</v>
       </c>
-      <c r="H58" s="89" t="s">
+      <c r="H58" s="82" t="s">
         <v>85</v>
       </c>
       <c r="I58" s="55"/>
     </row>
     <row r="59" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A59" s="87"/>
-      <c r="B59" s="69"/>
-      <c r="C59" s="69"/>
+      <c r="A59" s="70"/>
+      <c r="B59" s="73"/>
+      <c r="C59" s="73"/>
       <c r="D59" s="37" t="s">
         <v>146</v>
       </c>
@@ -3269,15 +3269,15 @@
       <c r="F59" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="G59" s="69"/>
-      <c r="H59" s="69"/>
+      <c r="G59" s="73"/>
+      <c r="H59" s="73"/>
       <c r="I59" s="41"/>
     </row>
     <row r="60" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="87"/>
-      <c r="B60" s="69"/>
-      <c r="C60" s="69"/>
-      <c r="D60" s="69" t="s">
+      <c r="A60" s="70"/>
+      <c r="B60" s="73"/>
+      <c r="C60" s="73"/>
+      <c r="D60" s="73" t="s">
         <v>158</v>
       </c>
       <c r="E60" s="11" t="s">
@@ -3286,117 +3286,117 @@
       <c r="F60" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="G60" s="69" t="s">
+      <c r="G60" s="73" t="s">
         <v>80</v>
       </c>
-      <c r="H60" s="69" t="s">
+      <c r="H60" s="73" t="s">
         <v>87</v>
       </c>
       <c r="I60" s="41"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="87"/>
-      <c r="B61" s="69"/>
-      <c r="C61" s="69"/>
-      <c r="D61" s="69"/>
+      <c r="A61" s="70"/>
+      <c r="B61" s="73"/>
+      <c r="C61" s="73"/>
+      <c r="D61" s="73"/>
       <c r="E61" s="11" t="s">
         <v>159</v>
       </c>
       <c r="F61" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="G61" s="69"/>
-      <c r="H61" s="69"/>
+      <c r="G61" s="73"/>
+      <c r="H61" s="73"/>
       <c r="I61" s="41"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="87"/>
-      <c r="B62" s="69"/>
-      <c r="C62" s="69"/>
-      <c r="D62" s="69"/>
+      <c r="A62" s="70"/>
+      <c r="B62" s="73"/>
+      <c r="C62" s="73"/>
+      <c r="D62" s="73"/>
       <c r="E62" s="11" t="s">
         <v>149</v>
       </c>
       <c r="F62" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="G62" s="69"/>
-      <c r="H62" s="69"/>
+      <c r="G62" s="73"/>
+      <c r="H62" s="73"/>
       <c r="I62" s="41"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="87"/>
-      <c r="B63" s="69"/>
-      <c r="C63" s="69"/>
-      <c r="D63" s="69"/>
+      <c r="A63" s="70"/>
+      <c r="B63" s="73"/>
+      <c r="C63" s="73"/>
+      <c r="D63" s="73"/>
       <c r="E63" s="11" t="s">
         <v>150</v>
       </c>
       <c r="F63" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="G63" s="69"/>
-      <c r="H63" s="69"/>
+      <c r="G63" s="73"/>
+      <c r="H63" s="73"/>
       <c r="I63" s="41"/>
     </row>
     <row r="64" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="87"/>
-      <c r="B64" s="69"/>
-      <c r="C64" s="69"/>
-      <c r="D64" s="69"/>
+      <c r="A64" s="70"/>
+      <c r="B64" s="73"/>
+      <c r="C64" s="73"/>
+      <c r="D64" s="73"/>
       <c r="E64" s="11" t="s">
         <v>151</v>
       </c>
       <c r="F64" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="G64" s="69"/>
-      <c r="H64" s="69"/>
+      <c r="G64" s="73"/>
+      <c r="H64" s="73"/>
       <c r="I64" s="41"/>
     </row>
     <row r="65" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="87"/>
-      <c r="B65" s="69"/>
-      <c r="C65" s="69"/>
-      <c r="D65" s="69"/>
+      <c r="A65" s="70"/>
+      <c r="B65" s="73"/>
+      <c r="C65" s="73"/>
+      <c r="D65" s="73"/>
       <c r="E65" s="11" t="s">
         <v>152</v>
       </c>
       <c r="F65" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="G65" s="69"/>
-      <c r="H65" s="69"/>
+      <c r="G65" s="73"/>
+      <c r="H65" s="73"/>
       <c r="I65" s="41"/>
     </row>
     <row r="66" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="87"/>
-      <c r="B66" s="69"/>
-      <c r="C66" s="69"/>
-      <c r="D66" s="69"/>
+      <c r="A66" s="70"/>
+      <c r="B66" s="73"/>
+      <c r="C66" s="73"/>
+      <c r="D66" s="73"/>
       <c r="E66" s="11" t="s">
         <v>153</v>
       </c>
       <c r="F66" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="G66" s="69"/>
-      <c r="H66" s="69"/>
+      <c r="G66" s="73"/>
+      <c r="H66" s="73"/>
       <c r="I66" s="41"/>
     </row>
     <row r="67" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="88"/>
-      <c r="B67" s="72"/>
-      <c r="C67" s="72"/>
-      <c r="D67" s="72"/>
+      <c r="A67" s="81"/>
+      <c r="B67" s="74"/>
+      <c r="C67" s="74"/>
+      <c r="D67" s="74"/>
       <c r="E67" s="24" t="s">
         <v>160</v>
       </c>
       <c r="F67" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="G67" s="72"/>
-      <c r="H67" s="72"/>
+      <c r="G67" s="74"/>
+      <c r="H67" s="74"/>
       <c r="I67" s="35"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -3510,6 +3510,58 @@
   </sheetData>
   <autoFilter ref="A1:I67"/>
   <mergeCells count="68">
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="B50:B57"/>
+    <mergeCell ref="C20:C49"/>
+    <mergeCell ref="C50:C57"/>
+    <mergeCell ref="D42:D44"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="G42:G44"/>
+    <mergeCell ref="H42:H44"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="D50:D52"/>
+    <mergeCell ref="G50:G52"/>
+    <mergeCell ref="H50:H52"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="G14:G18"/>
+    <mergeCell ref="H14:H18"/>
+    <mergeCell ref="B20:B49"/>
+    <mergeCell ref="D25:D31"/>
+    <mergeCell ref="G25:G31"/>
+    <mergeCell ref="H25:H31"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="D34:D41"/>
+    <mergeCell ref="G34:G41"/>
+    <mergeCell ref="H34:H41"/>
+    <mergeCell ref="G20:G24"/>
+    <mergeCell ref="H20:H24"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="G47:G49"/>
+    <mergeCell ref="A50:A57"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="H58:H59"/>
+    <mergeCell ref="D60:D67"/>
+    <mergeCell ref="G60:G67"/>
+    <mergeCell ref="H60:H67"/>
+    <mergeCell ref="C58:C67"/>
+    <mergeCell ref="A58:A67"/>
+    <mergeCell ref="B58:B67"/>
+    <mergeCell ref="D53:D57"/>
+    <mergeCell ref="G53:G57"/>
+    <mergeCell ref="H53:H57"/>
     <mergeCell ref="A20:A49"/>
     <mergeCell ref="C2:C6"/>
     <mergeCell ref="A2:A6"/>
@@ -3525,59 +3577,7 @@
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="C10:C13"/>
     <mergeCell ref="B10:B13"/>
-    <mergeCell ref="A50:A57"/>
-    <mergeCell ref="G58:G59"/>
-    <mergeCell ref="H58:H59"/>
-    <mergeCell ref="D60:D67"/>
-    <mergeCell ref="G60:G67"/>
-    <mergeCell ref="H60:H67"/>
-    <mergeCell ref="C58:C67"/>
-    <mergeCell ref="A58:A67"/>
-    <mergeCell ref="B58:B67"/>
-    <mergeCell ref="D53:D57"/>
-    <mergeCell ref="G53:G57"/>
-    <mergeCell ref="H53:H57"/>
-    <mergeCell ref="G14:G18"/>
-    <mergeCell ref="H14:H18"/>
-    <mergeCell ref="B20:B49"/>
-    <mergeCell ref="D25:D31"/>
-    <mergeCell ref="G25:G31"/>
-    <mergeCell ref="H25:H31"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="D34:D41"/>
-    <mergeCell ref="G34:G41"/>
-    <mergeCell ref="H34:H41"/>
-    <mergeCell ref="G20:G24"/>
-    <mergeCell ref="H20:H24"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="G47:G49"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="B50:B57"/>
-    <mergeCell ref="C20:C49"/>
-    <mergeCell ref="C50:C57"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="G42:G44"/>
-    <mergeCell ref="H42:H44"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="H45:H46"/>
-    <mergeCell ref="D50:D52"/>
-    <mergeCell ref="G50:G52"/>
-    <mergeCell ref="H50:H52"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I9" r:id="rId1"/>

</xml_diff>